<commit_message>
update LowHope Integration Test
</commit_message>
<xml_diff>
--- a/Document/IntegrationTest/LowHope Integration Test/IntegrationTest_BACK_ADMIN.xlsx
+++ b/Document/IntegrationTest/LowHope Integration Test/IntegrationTest_BACK_ADMIN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -570,7 +570,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="196">
   <si>
     <t>OJECT</t>
   </si>
@@ -1344,6 +1344,11 @@
   <si>
     <t>On Block Manager page
 1.Input value into data fields                                 2.Click on "Lưu" button                             3.Click on "Chắc chắn button"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Go to lowhope website
+1.Login
+2.Input email that doesn't exist in system</t>
   </si>
 </sst>
 </file>
@@ -1690,7 +1695,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1763,6 +1768,7 @@
     <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1790,7 +1796,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2072,10 +2080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:F5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2093,35 +2101,35 @@
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:10" ht="13.5" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="13.5" customHeight="1">
       <c r="A4" s="10" t="s">
@@ -2136,10 +2144,10 @@
       <c r="D4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" thickBot="1">
       <c r="A5" s="13">
@@ -2152,13 +2160,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="15">
-        <f>COUNTIF(F$10:H$1013,"N/A")</f>
+        <f>COUNTIF(F$10:H$1014,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="34">
         <v>4</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="51">
       <c r="A10" s="1" t="s">
@@ -2193,7 +2201,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="75">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="27" t="s">
         <v>178</v>
       </c>
       <c r="B11" s="3">
@@ -2221,7 +2229,7 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="75">
-      <c r="A12" s="27"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="3">
         <v>2</v>
       </c>
@@ -2246,19 +2254,19 @@
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="105">
-      <c r="A13" s="27"/>
+    <row r="13" spans="1:10" ht="90">
+      <c r="A13" s="28"/>
       <c r="B13" s="3">
         <v>3</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>16</v>
+        <v>195</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="18" t="s">
@@ -2272,7 +2280,7 @@
       </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="75">
+    <row r="14" spans="1:10" ht="105">
       <c r="A14" s="28"/>
       <c r="B14" s="3">
         <v>4</v>
@@ -2281,10 +2289,10 @@
         <v>11</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="18" t="s">
@@ -2298,9 +2306,38 @@
       </c>
       <c r="J14" s="5"/>
     </row>
+    <row r="15" spans="1:10" ht="75">
+      <c r="A15" s="29"/>
+      <c r="B15" s="3">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="6">
+        <v>43072</v>
+      </c>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="B16" s="36"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A11:A15"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
@@ -2339,35 +2376,35 @@
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="10" t="s">
@@ -2382,10 +2419,10 @@
       <c r="D4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="13">
@@ -2401,10 +2438,10 @@
         <f>COUNTIF(F$10:H$1014,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="34">
         <v>7</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="63.75">
       <c r="A10" s="1" t="s">
@@ -2439,7 +2476,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="114" customHeight="1">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="35" t="s">
         <v>178</v>
       </c>
       <c r="B11" s="3">
@@ -2467,7 +2504,7 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="114" customHeight="1">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="3">
         <v>2</v>
       </c>
@@ -2493,7 +2530,7 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="105">
-      <c r="A13" s="34"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -2519,7 +2556,7 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="105">
-      <c r="A14" s="34"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="3">
         <v>4</v>
       </c>
@@ -2545,7 +2582,7 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="105">
-      <c r="A15" s="34"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="3">
         <v>5</v>
       </c>
@@ -2571,7 +2608,7 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="105">
-      <c r="A16" s="34"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="3">
         <v>6</v>
       </c>
@@ -2597,7 +2634,7 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" ht="75">
-      <c r="A17" s="34"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="19">
         <v>7</v>
       </c>
@@ -2623,7 +2660,7 @@
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="34"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="3"/>
       <c r="C18" s="17"/>
       <c r="D18" s="7"/>
@@ -2635,7 +2672,7 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="34"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="21"/>
       <c r="C19" s="22"/>
       <c r="D19" s="23"/>
@@ -2647,7 +2684,7 @@
       <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="34"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="21"/>
       <c r="C20" s="22"/>
       <c r="D20" s="23"/>
@@ -2659,7 +2696,7 @@
       <c r="J20" s="24"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="34"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="21"/>
       <c r="C21" s="22"/>
       <c r="D21" s="23"/>
@@ -2671,7 +2708,7 @@
       <c r="J21" s="24"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="34"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="21"/>
       <c r="C22" s="22"/>
       <c r="D22" s="23"/>
@@ -2683,7 +2720,7 @@
       <c r="J22" s="24"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="34"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
       <c r="D23" s="23"/>
@@ -2695,7 +2732,7 @@
       <c r="J23" s="24"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="34"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
       <c r="D24" s="23"/>
@@ -2707,7 +2744,7 @@
       <c r="J24" s="24"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="34"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
       <c r="D25" s="23"/>
@@ -2719,7 +2756,7 @@
       <c r="J25" s="24"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="34"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="21"/>
       <c r="C26" s="22"/>
       <c r="D26" s="23"/>
@@ -2771,35 +2808,35 @@
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="10" t="s">
@@ -2814,10 +2851,10 @@
       <c r="D4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="13">
@@ -2833,10 +2870,10 @@
         <f>COUNTIF(F$10:H$1014,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="34">
         <v>5</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="63.75">
       <c r="A10" s="1" t="s">
@@ -2871,7 +2908,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="114" customHeight="1">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="35" t="s">
         <v>178</v>
       </c>
       <c r="B11" s="3">
@@ -2899,7 +2936,7 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="114" customHeight="1">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="3">
         <v>2</v>
       </c>
@@ -2925,7 +2962,7 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="135">
-      <c r="A13" s="34"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -2951,7 +2988,7 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="135">
-      <c r="A14" s="34"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="3">
         <v>4</v>
       </c>
@@ -2977,7 +3014,7 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="75">
-      <c r="A15" s="34"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="19">
         <v>5</v>
       </c>
@@ -3003,7 +3040,7 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="34"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="3"/>
       <c r="C16" s="17"/>
       <c r="D16" s="7"/>
@@ -3015,7 +3052,7 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="34"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="3"/>
       <c r="C17" s="17"/>
       <c r="D17" s="7"/>
@@ -3027,7 +3064,7 @@
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="34"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="3"/>
       <c r="C18" s="17"/>
       <c r="D18" s="7"/>
@@ -3039,7 +3076,7 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="34"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="21"/>
       <c r="C19" s="22"/>
       <c r="D19" s="23"/>
@@ -3051,7 +3088,7 @@
       <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="34"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="21"/>
       <c r="C20" s="22"/>
       <c r="D20" s="23"/>
@@ -3063,7 +3100,7 @@
       <c r="J20" s="24"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="34"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="21"/>
       <c r="C21" s="22"/>
       <c r="D21" s="23"/>
@@ -3075,7 +3112,7 @@
       <c r="J21" s="24"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="34"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="21"/>
       <c r="C22" s="22"/>
       <c r="D22" s="23"/>
@@ -3087,7 +3124,7 @@
       <c r="J22" s="24"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="34"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
       <c r="D23" s="23"/>
@@ -3099,7 +3136,7 @@
       <c r="J23" s="24"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="34"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
       <c r="D24" s="23"/>
@@ -3111,7 +3148,7 @@
       <c r="J24" s="24"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="34"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
       <c r="D25" s="23"/>
@@ -3123,7 +3160,7 @@
       <c r="J25" s="24"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="34"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="21"/>
       <c r="C26" s="22"/>
       <c r="D26" s="23"/>
@@ -3158,7 +3195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11:I13"/>
     </sheetView>
   </sheetViews>
@@ -3175,35 +3212,35 @@
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="10" t="s">
@@ -3218,10 +3255,10 @@
       <c r="D4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="13">
@@ -3237,10 +3274,10 @@
         <f>COUNTIF(F$10:H$1014,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="34">
         <v>3</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="63.75">
       <c r="A10" s="1" t="s">
@@ -3275,7 +3312,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="153.75" customHeight="1">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="35" t="s">
         <v>178</v>
       </c>
       <c r="B11" s="3">
@@ -3303,7 +3340,7 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="152.25" customHeight="1">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="3">
         <v>2</v>
       </c>
@@ -3329,7 +3366,7 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="135">
-      <c r="A13" s="34"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -3355,7 +3392,7 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="34"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="3"/>
       <c r="C14" s="17"/>
       <c r="D14" s="7"/>
@@ -3367,7 +3404,7 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="34"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="19"/>
       <c r="C15" s="20"/>
       <c r="D15" s="7"/>
@@ -3379,7 +3416,7 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="34"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="3"/>
       <c r="C16" s="17"/>
       <c r="D16" s="7"/>
@@ -3391,7 +3428,7 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="34"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="3"/>
       <c r="C17" s="17"/>
       <c r="D17" s="7"/>
@@ -3403,7 +3440,7 @@
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="34"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="3"/>
       <c r="C18" s="17"/>
       <c r="D18" s="7"/>
@@ -3415,7 +3452,7 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="34"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="21"/>
       <c r="C19" s="22"/>
       <c r="D19" s="23"/>
@@ -3427,7 +3464,7 @@
       <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="34"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="21"/>
       <c r="C20" s="22"/>
       <c r="D20" s="23"/>
@@ -3439,7 +3476,7 @@
       <c r="J20" s="24"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="34"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="21"/>
       <c r="C21" s="22"/>
       <c r="D21" s="23"/>
@@ -3451,7 +3488,7 @@
       <c r="J21" s="24"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="34"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="21"/>
       <c r="C22" s="22"/>
       <c r="D22" s="23"/>
@@ -3463,7 +3500,7 @@
       <c r="J22" s="24"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="34"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
       <c r="D23" s="23"/>
@@ -3475,7 +3512,7 @@
       <c r="J23" s="24"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="34"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
       <c r="D24" s="23"/>
@@ -3487,7 +3524,7 @@
       <c r="J24" s="24"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="34"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
       <c r="D25" s="23"/>
@@ -3499,7 +3536,7 @@
       <c r="J25" s="24"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="34"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="21"/>
       <c r="C26" s="22"/>
       <c r="D26" s="23"/>
@@ -3551,35 +3588,35 @@
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="10" t="s">
@@ -3594,10 +3631,10 @@
       <c r="D4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="13">
@@ -3613,10 +3650,10 @@
         <f>COUNTIF(F$10:H$1015,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="34">
         <v>5</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="63.75">
       <c r="A10" s="1" t="s">
@@ -3651,7 +3688,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="60">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="35" t="s">
         <v>178</v>
       </c>
       <c r="B11" s="3">
@@ -3679,7 +3716,7 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="195">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="3">
         <v>2</v>
       </c>
@@ -3705,7 +3742,7 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="210">
-      <c r="A13" s="34"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -3731,7 +3768,7 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="105">
-      <c r="A14" s="34"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="3">
         <v>4</v>
       </c>
@@ -3757,7 +3794,7 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="75">
-      <c r="A15" s="34"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="19">
         <v>5</v>
       </c>
@@ -3823,35 +3860,35 @@
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="10" t="s">
@@ -3866,10 +3903,10 @@
       <c r="D4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="13">
@@ -3885,10 +3922,10 @@
         <f>COUNTIF(F$10:H$1013,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="34">
         <v>5</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="63.75">
       <c r="A10" s="1" t="s">
@@ -3923,7 +3960,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="90">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="27" t="s">
         <v>178</v>
       </c>
       <c r="B11" s="3">
@@ -3951,7 +3988,7 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="120">
-      <c r="A12" s="27"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="3">
         <v>2</v>
       </c>
@@ -3977,7 +4014,7 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="135">
-      <c r="A13" s="27"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -4003,7 +4040,7 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="75">
-      <c r="A14" s="27"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="19">
         <v>4</v>
       </c>
@@ -4029,7 +4066,7 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="75">
-      <c r="A15" s="28"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="19">
         <v>5</v>
       </c>
@@ -4056,12 +4093,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A11:A15"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="A11:A15"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F2">
@@ -4095,35 +4132,35 @@
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="10" t="s">
@@ -4138,10 +4175,10 @@
       <c r="D4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="13">
@@ -4157,10 +4194,10 @@
         <f>COUNTIF(F$10:H$1013,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="34">
         <v>9</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="63.75">
       <c r="A10" s="1" t="s">
@@ -4195,7 +4232,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="60">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="27" t="s">
         <v>178</v>
       </c>
       <c r="B11" s="3">
@@ -4223,7 +4260,7 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="75">
-      <c r="A12" s="27"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="3">
         <v>2</v>
       </c>
@@ -4249,7 +4286,7 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="75">
-      <c r="A13" s="27"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -4275,7 +4312,7 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="75">
-      <c r="A14" s="27"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="19">
         <v>4</v>
       </c>
@@ -4301,7 +4338,7 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="75">
-      <c r="A15" s="27"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="19">
         <v>5</v>
       </c>
@@ -4327,7 +4364,7 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="75">
-      <c r="A16" s="27"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="19">
         <v>6</v>
       </c>
@@ -4353,7 +4390,7 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" ht="75">
-      <c r="A17" s="27"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="19">
         <v>7</v>
       </c>
@@ -4379,7 +4416,7 @@
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" ht="75">
-      <c r="A18" s="27"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="19">
         <v>8</v>
       </c>
@@ -4405,7 +4442,7 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" ht="75">
-      <c r="A19" s="28"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="19">
         <v>9</v>
       </c>
@@ -4471,35 +4508,35 @@
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="10" t="s">
@@ -4514,10 +4551,10 @@
       <c r="D4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="13">
@@ -4533,10 +4570,10 @@
         <f>COUNTIF(F$10:H$1015,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="34">
         <v>6</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="63.75">
       <c r="A10" s="1" t="s">
@@ -4571,7 +4608,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="114" customHeight="1">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="27" t="s">
         <v>178</v>
       </c>
       <c r="B11" s="3">
@@ -4599,7 +4636,7 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="114" customHeight="1">
-      <c r="A12" s="27"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="3">
         <v>2</v>
       </c>
@@ -4625,7 +4662,7 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="90">
-      <c r="A13" s="27"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -4651,7 +4688,7 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="105">
-      <c r="A14" s="27"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="3">
         <v>4</v>
       </c>
@@ -4677,7 +4714,7 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="90">
-      <c r="A15" s="27"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="3">
         <v>5</v>
       </c>
@@ -4703,7 +4740,7 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="75">
-      <c r="A16" s="28"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="19">
         <v>6</v>
       </c>
@@ -4769,35 +4806,35 @@
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="10" t="s">
@@ -4812,10 +4849,10 @@
       <c r="D4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="13">
@@ -4831,10 +4868,10 @@
         <f>COUNTIF(F$10:H$1015,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="34">
         <v>7</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="63.75">
       <c r="A10" s="1" t="s">
@@ -4869,7 +4906,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="114" customHeight="1">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="27" t="s">
         <v>178</v>
       </c>
       <c r="B11" s="3">
@@ -4897,7 +4934,7 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="114" customHeight="1">
-      <c r="A12" s="27"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="3">
         <v>2</v>
       </c>
@@ -4923,7 +4960,7 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="90">
-      <c r="A13" s="27"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -4949,7 +4986,7 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="60">
-      <c r="A14" s="27"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="3">
         <v>4</v>
       </c>
@@ -4975,7 +5012,7 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="60">
-      <c r="A15" s="27"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="3">
         <v>5</v>
       </c>
@@ -5001,7 +5038,7 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="60">
-      <c r="A16" s="27"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="3">
         <v>6</v>
       </c>
@@ -5027,7 +5064,7 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" ht="60">
-      <c r="A17" s="28"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="3">
         <v>7</v>
       </c>
@@ -5093,35 +5130,35 @@
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="10" t="s">
@@ -5136,10 +5173,10 @@
       <c r="D4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="13">
@@ -5155,10 +5192,10 @@
         <f>COUNTIF(F$10:H$1015,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E5" s="33">
-        <v>10</v>
-      </c>
-      <c r="F5" s="33"/>
+      <c r="E5" s="34">
+        <v>10</v>
+      </c>
+      <c r="F5" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="63.75">
       <c r="A10" s="1" t="s">
@@ -5193,7 +5230,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="114" customHeight="1">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="27" t="s">
         <v>178</v>
       </c>
       <c r="B11" s="3">
@@ -5221,7 +5258,7 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="114" customHeight="1">
-      <c r="A12" s="27"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="3">
         <v>2</v>
       </c>
@@ -5247,7 +5284,7 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="75">
-      <c r="A13" s="27"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -5273,7 +5310,7 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="75">
-      <c r="A14" s="27"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="3">
         <v>4</v>
       </c>
@@ -5299,7 +5336,7 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="75">
-      <c r="A15" s="27"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="3">
         <v>5</v>
       </c>
@@ -5325,7 +5362,7 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="120">
-      <c r="A16" s="27"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="3">
         <v>6</v>
       </c>
@@ -5351,7 +5388,7 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" ht="75">
-      <c r="A17" s="27"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="3">
         <v>7</v>
       </c>
@@ -5377,7 +5414,7 @@
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" ht="105">
-      <c r="A18" s="27"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="3">
         <v>8</v>
       </c>
@@ -5403,7 +5440,7 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" ht="75">
-      <c r="A19" s="27"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="3">
         <v>9</v>
       </c>
@@ -5429,7 +5466,7 @@
       <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10" ht="75">
-      <c r="A20" s="28"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="3">
         <v>10</v>
       </c>
@@ -5495,35 +5532,35 @@
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="10" t="s">
@@ -5538,10 +5575,10 @@
       <c r="D4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="13">
@@ -5557,10 +5594,10 @@
         <f>COUNTIF(F$10:H$1014,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="34">
         <v>16</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="63.75">
       <c r="A10" s="1" t="s">
@@ -5595,7 +5632,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="114" customHeight="1">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="35" t="s">
         <v>178</v>
       </c>
       <c r="B11" s="3">
@@ -5623,7 +5660,7 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="114" customHeight="1">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="3">
         <v>2</v>
       </c>
@@ -5649,7 +5686,7 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="150">
-      <c r="A13" s="34"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -5675,7 +5712,7 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="180">
-      <c r="A14" s="34"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="3">
         <v>4</v>
       </c>
@@ -5701,7 +5738,7 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="150">
-      <c r="A15" s="34"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="3">
         <v>5</v>
       </c>
@@ -5727,7 +5764,7 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="105">
-      <c r="A16" s="34"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="3">
         <v>6</v>
       </c>
@@ -5753,7 +5790,7 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" ht="90">
-      <c r="A17" s="34"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="3">
         <v>7</v>
       </c>
@@ -5779,7 +5816,7 @@
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" ht="75">
-      <c r="A18" s="34"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="3">
         <v>8</v>
       </c>
@@ -5805,7 +5842,7 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" ht="90">
-      <c r="A19" s="34"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="3">
         <v>9</v>
       </c>
@@ -5831,7 +5868,7 @@
       <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10" ht="90">
-      <c r="A20" s="34"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="3">
         <v>10</v>
       </c>
@@ -5857,7 +5894,7 @@
       <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:10" ht="90">
-      <c r="A21" s="34"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="3">
         <v>11</v>
       </c>
@@ -5883,7 +5920,7 @@
       <c r="J21" s="5"/>
     </row>
     <row r="22" spans="1:10" ht="90">
-      <c r="A22" s="34"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="3">
         <v>12</v>
       </c>
@@ -5909,7 +5946,7 @@
       <c r="J22" s="5"/>
     </row>
     <row r="23" spans="1:10" ht="90">
-      <c r="A23" s="34"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="3">
         <v>13</v>
       </c>
@@ -5935,7 +5972,7 @@
       <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" ht="90">
-      <c r="A24" s="34"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="3">
         <v>14</v>
       </c>
@@ -5961,7 +5998,7 @@
       <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" ht="90">
-      <c r="A25" s="34"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="3">
         <v>15</v>
       </c>
@@ -5987,7 +6024,7 @@
       <c r="J25" s="5"/>
     </row>
     <row r="26" spans="1:10" ht="90">
-      <c r="A26" s="34"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="3">
         <v>16</v>
       </c>
@@ -6013,7 +6050,7 @@
       <c r="J26" s="5"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="34"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="19"/>
       <c r="C27" s="20"/>
       <c r="D27" s="7"/>
@@ -6025,17 +6062,17 @@
       <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A11:A27"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="A11:A27"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F2">
@@ -6069,35 +6106,35 @@
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="10" t="s">
@@ -6112,10 +6149,10 @@
       <c r="D4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="13">
@@ -6131,10 +6168,10 @@
         <f>COUNTIF(F$10:H$1014,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="34">
         <v>9</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="63.75">
       <c r="A10" s="1" t="s">
@@ -6169,7 +6206,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="114" customHeight="1">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="35" t="s">
         <v>178</v>
       </c>
       <c r="B11" s="3">
@@ -6197,7 +6234,7 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="114" customHeight="1">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="3">
         <v>2</v>
       </c>
@@ -6223,7 +6260,7 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="105">
-      <c r="A13" s="34"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -6249,7 +6286,7 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="105">
-      <c r="A14" s="34"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="3">
         <v>4</v>
       </c>
@@ -6275,7 +6312,7 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="105">
-      <c r="A15" s="34"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="3">
         <v>5</v>
       </c>
@@ -6301,7 +6338,7 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="105">
-      <c r="A16" s="34"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="3">
         <v>6</v>
       </c>
@@ -6327,7 +6364,7 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" ht="105">
-      <c r="A17" s="34"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="3">
         <v>7</v>
       </c>
@@ -6353,7 +6390,7 @@
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" ht="180">
-      <c r="A18" s="34"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="3">
         <v>8</v>
       </c>
@@ -6379,7 +6416,7 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" ht="75">
-      <c r="A19" s="34"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="19">
         <v>9</v>
       </c>
@@ -6405,7 +6442,7 @@
       <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="34"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="21"/>
       <c r="C20" s="22"/>
       <c r="D20" s="23"/>
@@ -6417,7 +6454,7 @@
       <c r="J20" s="24"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="34"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="21"/>
       <c r="C21" s="22"/>
       <c r="D21" s="23"/>
@@ -6429,7 +6466,7 @@
       <c r="J21" s="24"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="34"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="21"/>
       <c r="C22" s="22"/>
       <c r="D22" s="23"/>
@@ -6441,7 +6478,7 @@
       <c r="J22" s="24"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="34"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
       <c r="D23" s="23"/>
@@ -6453,7 +6490,7 @@
       <c r="J23" s="24"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="34"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
       <c r="D24" s="23"/>
@@ -6465,7 +6502,7 @@
       <c r="J24" s="24"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="34"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
       <c r="D25" s="23"/>
@@ -6477,7 +6514,7 @@
       <c r="J25" s="24"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="34"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="21"/>
       <c r="C26" s="22"/>
       <c r="D26" s="23"/>

</xml_diff>